<commit_message>
Add REGCV1 data to case ieee123
</commit_message>
<xml_diff>
--- a/ams/cases/ieee123/ieee123.xlsx
+++ b/ams/cases/ieee123/ieee123.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\buxin\andes\bshe\stability_VIS\ams_for_vis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee123/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160EE363-8BCA-494C-B38C-7682308E321D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB133220-1218-8047-8B19-0B03412C9F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bus" sheetId="1" r:id="rId1"/>
-    <sheet name="PV" sheetId="3" r:id="rId2"/>
-    <sheet name="PQ" sheetId="2" r:id="rId3"/>
-    <sheet name="Slack" sheetId="4" r:id="rId4"/>
-    <sheet name="Line" sheetId="5" r:id="rId5"/>
-    <sheet name="GCost" sheetId="14" r:id="rId6"/>
+    <sheet name="Summary" sheetId="15" r:id="rId1"/>
+    <sheet name="Bus" sheetId="1" r:id="rId2"/>
+    <sheet name="PV" sheetId="3" r:id="rId3"/>
+    <sheet name="PQ" sheetId="2" r:id="rId4"/>
+    <sheet name="Slack" sheetId="4" r:id="rId5"/>
+    <sheet name="Line" sheetId="5" r:id="rId6"/>
+    <sheet name="GCost" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="614">
   <si>
     <t>idx</t>
   </si>
@@ -1859,13 +1860,34 @@
   </si>
   <si>
     <t>GCOST_11</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>comment2</t>
+  </si>
+  <si>
+    <t>comment3</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>IEEE 123-bus test case</t>
+  </si>
+  <si>
+    <t>for OPF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1887,6 +1909,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1896,7 +1933,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1919,11 +1956,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1934,6 +1997,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2237,6 +2310,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DBA7FE-37BF-AE44-98CD-671473739CD3}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="E2" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N118"/>
   <sheetViews>
@@ -2245,9 +2365,9 @@
       <selection pane="bottomLeft" activeCell="A116" sqref="A116:XFD118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2291,7 +2411,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2332,7 +2452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2373,7 +2493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2414,7 +2534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2455,7 +2575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2496,7 +2616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2537,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2578,7 +2698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2619,7 +2739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2660,7 +2780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2701,7 +2821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2742,7 +2862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2783,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2824,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2865,7 +2985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2906,7 +3026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2947,7 +3067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2988,7 +3108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3029,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3070,7 +3190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -3111,7 +3231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -3152,7 +3272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -3193,7 +3313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3234,7 +3354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3275,7 +3395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -3316,7 +3436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -3357,7 +3477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -3398,7 +3518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3439,7 +3559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3480,7 +3600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3521,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3562,7 +3682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3603,7 +3723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3644,7 +3764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3685,7 +3805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3726,7 +3846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3767,7 +3887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3808,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3849,7 +3969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3890,7 +4010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3931,7 +4051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3972,7 +4092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -4013,7 +4133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -4054,7 +4174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4095,7 +4215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4136,7 +4256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4177,7 +4297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4218,7 +4338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4259,7 +4379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4300,7 +4420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4341,7 +4461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4382,7 +4502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4423,7 +4543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4464,7 +4584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4505,7 +4625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4546,7 +4666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4587,7 +4707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4628,7 +4748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4669,7 +4789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4710,7 +4830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -4751,7 +4871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4792,7 +4912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4833,7 +4953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4874,7 +4994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -4915,7 +5035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -4956,7 +5076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -4997,7 +5117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -5038,7 +5158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -5079,7 +5199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -5120,7 +5240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -5161,7 +5281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -5202,7 +5322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -5243,7 +5363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -5284,7 +5404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -5325,7 +5445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -5366,7 +5486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -5407,7 +5527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -5448,7 +5568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -5489,7 +5609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -5530,7 +5650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -5571,7 +5691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -5612,7 +5732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -5653,7 +5773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -5694,7 +5814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -5735,7 +5855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -5776,7 +5896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -5817,7 +5937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -5858,7 +5978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -5899,7 +6019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -5940,7 +6060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -5981,7 +6101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -6022,7 +6142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -6063,7 +6183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -6104,7 +6224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -6145,7 +6265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -6186,7 +6306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -6227,7 +6347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -6268,7 +6388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -6309,7 +6429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -6350,7 +6470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -6391,7 +6511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -6432,7 +6552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -6473,7 +6593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -6514,7 +6634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -6555,7 +6675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -6596,7 +6716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -6637,7 +6757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -6678,7 +6798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -6719,7 +6839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -6760,7 +6880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -6801,7 +6921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -6842,7 +6962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -6883,7 +7003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -6924,7 +7044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -6965,7 +7085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -7006,7 +7126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -7047,7 +7167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -7093,7 +7213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S11"/>
   <sheetViews>
@@ -7102,9 +7222,9 @@
       <selection pane="bottomLeft" activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -7163,7 +7283,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>565</v>
       </c>
@@ -7219,7 +7339,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>566</v>
       </c>
@@ -7275,7 +7395,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>567</v>
       </c>
@@ -7331,7 +7451,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>568</v>
       </c>
@@ -7387,7 +7507,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>569</v>
       </c>
@@ -7443,7 +7563,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>570</v>
       </c>
@@ -7499,7 +7619,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>571</v>
       </c>
@@ -7555,7 +7675,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>572</v>
       </c>
@@ -7611,7 +7731,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>573</v>
       </c>
@@ -7667,7 +7787,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>574</v>
       </c>
@@ -7729,7 +7849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K87"/>
   <sheetViews>
@@ -7738,9 +7858,9 @@
       <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -7775,7 +7895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -7807,7 +7927,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -7839,7 +7959,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -7871,7 +7991,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -7903,7 +8023,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -7935,7 +8055,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -7967,7 +8087,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -7999,7 +8119,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -8031,7 +8151,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -8063,7 +8183,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -8095,7 +8215,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -8127,7 +8247,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -8159,7 +8279,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -8191,7 +8311,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -8223,7 +8343,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -8255,7 +8375,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -8287,7 +8407,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -8319,7 +8439,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -8351,7 +8471,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -8383,7 +8503,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -8415,7 +8535,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -8447,7 +8567,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -8479,7 +8599,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -8511,7 +8631,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -8543,7 +8663,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -8575,7 +8695,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -8607,7 +8727,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -8639,7 +8759,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -8671,7 +8791,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -8703,7 +8823,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -8735,7 +8855,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -8767,7 +8887,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -8799,7 +8919,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -8831,7 +8951,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -8863,7 +8983,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -8895,7 +9015,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -8927,7 +9047,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -8959,7 +9079,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -8991,7 +9111,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -9023,7 +9143,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -9055,7 +9175,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -9087,7 +9207,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -9119,7 +9239,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -9151,7 +9271,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -9183,7 +9303,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -9215,7 +9335,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -9247,7 +9367,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -9279,7 +9399,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -9311,7 +9431,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -9343,7 +9463,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -9375,7 +9495,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -9407,7 +9527,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -9439,7 +9559,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -9471,7 +9591,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -9503,7 +9623,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -9535,7 +9655,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -9567,7 +9687,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -9599,7 +9719,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -9631,7 +9751,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -9663,7 +9783,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -9695,7 +9815,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -9727,7 +9847,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -9759,7 +9879,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -9791,7 +9911,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -9823,7 +9943,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -9855,7 +9975,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -9887,7 +10007,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -9919,7 +10039,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -9951,7 +10071,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -9983,7 +10103,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -10015,7 +10135,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -10047,7 +10167,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -10079,7 +10199,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -10111,7 +10231,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -10143,7 +10263,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -10175,7 +10295,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -10207,7 +10327,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -10239,7 +10359,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -10271,7 +10391,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -10303,7 +10423,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -10335,7 +10455,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -10367,7 +10487,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -10399,7 +10519,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -10431,7 +10551,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -10463,7 +10583,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -10495,7 +10615,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -10525,143 +10645,6 @@
       </c>
       <c r="J87">
         <v>0.8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:T2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="E2" s="2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2">
-        <v>4.16</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0.65</v>
-      </c>
-      <c r="K2" s="2">
-        <v>2</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="M2" s="2">
-        <v>2</v>
-      </c>
-      <c r="N2" s="2">
-        <v>-2</v>
-      </c>
-      <c r="O2" s="2">
-        <v>1</v>
-      </c>
-      <c r="P2" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="T2" s="2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -10670,6 +10653,143 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4.16</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="M2" s="2">
+        <v>2</v>
+      </c>
+      <c r="N2" s="2">
+        <v>-2</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA117"/>
   <sheetViews>
@@ -10678,12 +10798,12 @@
       <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="15.41796875" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -10766,7 +10886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -10840,7 +10960,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -10914,7 +11034,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -10988,7 +11108,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -11062,7 +11182,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -11136,7 +11256,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -11210,7 +11330,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -11284,7 +11404,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -11358,7 +11478,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -11432,7 +11552,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -11506,7 +11626,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -11580,7 +11700,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -11654,7 +11774,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -11728,7 +11848,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -11802,7 +11922,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -11876,7 +11996,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -11950,7 +12070,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -12024,7 +12144,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -12098,7 +12218,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -12172,7 +12292,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -12246,7 +12366,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -12320,7 +12440,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -12394,7 +12514,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -12468,7 +12588,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -12542,7 +12662,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -12616,7 +12736,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -12690,7 +12810,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -12764,7 +12884,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -12838,7 +12958,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -12912,7 +13032,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -12986,7 +13106,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -13060,7 +13180,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -13134,7 +13254,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -13208,7 +13328,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -13282,7 +13402,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -13356,7 +13476,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -13430,7 +13550,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -13504,7 +13624,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -13578,7 +13698,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -13652,7 +13772,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -13726,7 +13846,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -13800,7 +13920,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -13874,7 +13994,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -13948,7 +14068,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -14022,7 +14142,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -14096,7 +14216,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -14170,7 +14290,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -14244,7 +14364,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -14318,7 +14438,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -14392,7 +14512,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -14466,7 +14586,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -14540,7 +14660,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -14614,7 +14734,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -14688,7 +14808,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -14762,7 +14882,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -14836,7 +14956,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -14910,7 +15030,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -14984,7 +15104,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -15058,7 +15178,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -15132,7 +15252,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -15206,7 +15326,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -15280,7 +15400,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -15354,7 +15474,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -15428,7 +15548,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -15502,7 +15622,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -15576,7 +15696,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -15650,7 +15770,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -15724,7 +15844,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -15798,7 +15918,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -15872,7 +15992,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -15946,7 +16066,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -16020,7 +16140,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -16094,7 +16214,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -16168,7 +16288,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -16242,7 +16362,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -16316,7 +16436,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -16390,7 +16510,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -16464,7 +16584,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -16538,7 +16658,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -16612,7 +16732,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -16686,7 +16806,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -16760,7 +16880,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -16834,7 +16954,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -16908,7 +17028,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -16982,7 +17102,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -17056,7 +17176,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -17130,7 +17250,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -17204,7 +17324,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -17278,7 +17398,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -17352,7 +17472,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -17426,7 +17546,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -17500,7 +17620,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -17574,7 +17694,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -17648,7 +17768,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -17722,7 +17842,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -17796,7 +17916,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -17870,7 +17990,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -17944,7 +18064,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -18018,7 +18138,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -18092,7 +18212,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -18166,7 +18286,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -18240,7 +18360,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -18314,7 +18434,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -18388,7 +18508,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -18462,7 +18582,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -18536,7 +18656,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -18610,7 +18730,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -18684,7 +18804,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -18758,7 +18878,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -18832,7 +18952,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -18906,7 +19026,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -18980,7 +19100,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -19054,7 +19174,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -19128,7 +19248,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -19202,7 +19322,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -19276,7 +19396,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -19355,7 +19475,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D71AA9-7122-4644-932B-DB8CEB0A118F}">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -19363,12 +19483,12 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="11.7890625" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -19397,7 +19517,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>565</v>
       </c>
@@ -19426,7 +19546,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>566</v>
       </c>
@@ -19455,7 +19575,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>567</v>
       </c>
@@ -19484,7 +19604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>568</v>
       </c>
@@ -19513,7 +19633,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>569</v>
       </c>
@@ -19542,7 +19662,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>570</v>
       </c>
@@ -19571,7 +19691,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>571</v>
       </c>
@@ -19600,7 +19720,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>572</v>
       </c>
@@ -19629,7 +19749,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>573</v>
       </c>
@@ -19658,7 +19778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>574</v>
       </c>
@@ -19687,7 +19807,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>600</v>
       </c>

</xml_diff>